<commit_message>
Project finished, no Unity build
</commit_message>
<xml_diff>
--- a/documentation/IGA Final Asset List.xlsx
+++ b/documentation/IGA Final Asset List.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="75">
   <si>
     <t>Event Name</t>
   </si>
@@ -40,6 +40,9 @@
     <t>menu sound</t>
   </si>
   <si>
+    <t>done</t>
+  </si>
+  <si>
     <t>buttonPress</t>
   </si>
   <si>
@@ -169,6 +172,9 @@
     <t>ambient loop</t>
   </si>
   <si>
+    <t>removed</t>
+  </si>
+  <si>
     <t>dogGowl2</t>
   </si>
   <si>
@@ -215,6 +221,21 @@
   </si>
   <si>
     <t>effect when player runs into rat</t>
+  </si>
+  <si>
+    <t>Ambience</t>
+  </si>
+  <si>
+    <t>ambience1</t>
+  </si>
+  <si>
+    <t>ambient traffic noises</t>
+  </si>
+  <si>
+    <t>ambience2</t>
+  </si>
+  <si>
+    <t>ambience3</t>
   </si>
 </sst>
 </file>
@@ -262,7 +283,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border/>
     <border>
       <bottom style="thin">
@@ -287,11 +308,19 @@
         <color rgb="FF000000"/>
       </top>
     </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -316,16 +345,20 @@
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -578,342 +611,455 @@
       <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="F2" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="5"/>
       <c r="B3" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>8</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="5"/>
       <c r="B4" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5"/>
       <c r="B5" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="5"/>
       <c r="B6" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5"/>
       <c r="B7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>18</v>
+      <c r="F7" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="5"/>
       <c r="B8" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>8</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5"/>
       <c r="B9" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="5"/>
       <c r="B10" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5"/>
       <c r="B11" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="5"/>
       <c r="B12" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5"/>
       <c r="B13" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="5"/>
       <c r="B14" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="7"/>
       <c r="B15" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" s="10"/>
+        <v>41</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="11" t="s">
-        <v>41</v>
+      <c r="A16" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="12" t="s">
         <v>43</v>
       </c>
+      <c r="C16" s="11" t="s">
+        <v>44</v>
+      </c>
       <c r="D16" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="5"/>
       <c r="B17" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="7"/>
       <c r="B18" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
+        <v>14</v>
+      </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="9" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" s="11" t="s">
-        <v>48</v>
+      <c r="A19" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="5"/>
       <c r="B20" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>51</v>
+      <c r="F20" s="4" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="7"/>
       <c r="B21" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="12"/>
+      <c r="F21" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
     </row>
     <row r="22">
-      <c r="A22" s="11" t="s">
-        <v>55</v>
+      <c r="A22" s="10" t="s">
+        <v>57</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>59</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="5"/>
       <c r="B23" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="7"/>
       <c r="B24" s="8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
+        <v>14</v>
+      </c>
+      <c r="E24" s="12"/>
+      <c r="F24" s="9" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" s="11" t="s">
-        <v>62</v>
+      <c r="A25" s="10" t="s">
+        <v>64</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="5"/>
       <c r="B26" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="5"/>
       <c r="B27" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="5"/>
+      <c r="A28" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" s="15"/>
+      <c r="F28" s="11" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="5"/>
+      <c r="B29" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="5"/>
+      <c r="B30" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="5"/>

</xml_diff>